<commit_message>
Duplicates removed and same parts in different spaces combined.
</commit_message>
<xml_diff>
--- a/PartsList.xlsx
+++ b/PartsList.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/engs1793_ox_ac_uk/Documents/4pi_workspace/Git/CAD-files-master/CAD-files-master/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/engs1793_ox_ac_uk/Documents/4pi_workspace/Git/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7584"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10092"/>
   </bookViews>
   <sheets>
     <sheet name="4Pi-SMS partlist" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="506">
   <si>
     <t>Category</t>
   </si>
@@ -881,9 +881,6 @@
     <t>LM2XY/M - Translating Lens Mount for Ø2" Optics, 1 Retaining Ring Included, Metric</t>
   </si>
   <si>
-    <t>Dovetail Rail Carrier, 1/4" (M6) Counterbore</t>
-  </si>
-  <si>
     <t>RLA450_M</t>
   </si>
   <si>
@@ -891,9 +888,6 @@
   </si>
   <si>
     <t>KM200</t>
-  </si>
-  <si>
-    <t>Kinematic Mirror Mount for Ø2" Optics</t>
   </si>
   <si>
     <t>RC3</t>
@@ -1048,12 +1042,6 @@
 with ø 25 mm / 25.4 mm (1"), deflection to the left</t>
   </si>
   <si>
-    <t>RC12FC-P01</t>
-  </si>
-  <si>
-    <t>Protected Silver Reflective Collimator, 450 nm - 20 µm, Ø12 mm Beam, FC/P</t>
-  </si>
-  <si>
     <t>K5X1</t>
   </si>
   <si>
@@ -1298,9 +1286,6 @@
   </si>
   <si>
     <t xml:space="preserve">RC12FC-P01 - Protected Silver Reflective Collimator, 450 nm - 20 µm, Ø12 mm Beam, FC/PC </t>
-  </si>
-  <si>
-    <t>£724.76</t>
   </si>
   <si>
     <t>SM15RR</t>
@@ -1559,20 +1544,17 @@
     <t>Collimated Laser-Diode-Pumped DPSS Laser Module, 532 nm, 0.9 mW, Round Beam, Ø11 mm Housing</t>
   </si>
   <si>
-    <t>PELCO SEMClip™ Clips, pkg/10</t>
-  </si>
-  <si>
-    <t>Ted Pella</t>
-  </si>
-  <si>
-    <t>PELCO SEMClip™ Screws, Brass, M2 x 3mm length, pkg/10</t>
+    <t>https://www.tedpella.com/SEM_html/SEMclip.htm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1599,6 +1581,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1623,10 +1611,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1662,8 +1651,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1879,8 +1871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U954"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="C184" sqref="C184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2403,11 +2395,11 @@
         <v>16</v>
       </c>
       <c r="E20" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" ref="F20:F22" si="4">E20*H20</f>
-        <v>17.93</v>
+        <v>89.65</v>
       </c>
       <c r="H20" s="1">
         <v>17.93</v>
@@ -4750,21 +4742,11 @@
       <c r="U114" s="12"/>
     </row>
     <row r="115" spans="1:21" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="16" t="s">
-        <v>280</v>
-      </c>
-      <c r="B115" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C115" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="D115" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E115" s="16">
-        <v>5</v>
-      </c>
+      <c r="A115" s="16"/>
+      <c r="B115" s="16"/>
+      <c r="C115" s="16"/>
+      <c r="D115" s="16"/>
+      <c r="E115" s="16"/>
       <c r="F115" s="12"/>
       <c r="G115" s="12"/>
       <c r="H115" s="12"/>
@@ -4787,10 +4769,10 @@
         <v>280</v>
       </c>
       <c r="B116" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="C116" s="16" t="s">
         <v>286</v>
-      </c>
-      <c r="C116" s="16" t="s">
-        <v>287</v>
       </c>
       <c r="D116" s="16" t="s">
         <v>16</v>
@@ -4816,21 +4798,11 @@
       <c r="U116" s="12"/>
     </row>
     <row r="117" spans="1:21" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="16" t="s">
-        <v>280</v>
-      </c>
-      <c r="B117" s="16" t="s">
-        <v>288</v>
-      </c>
-      <c r="C117" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="D117" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E117" s="16">
-        <v>1</v>
-      </c>
+      <c r="A117" s="16"/>
+      <c r="B117" s="16"/>
+      <c r="C117" s="16"/>
+      <c r="D117" s="16"/>
+      <c r="E117" s="16"/>
       <c r="F117" s="12"/>
       <c r="G117" s="12"/>
       <c r="H117" s="12"/>
@@ -4853,10 +4825,10 @@
         <v>280</v>
       </c>
       <c r="B118" s="16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C118" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D118" s="16" t="s">
         <v>16</v>
@@ -4886,10 +4858,10 @@
         <v>280</v>
       </c>
       <c r="B119" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D119" s="16" t="s">
         <v>16</v>
@@ -4919,10 +4891,10 @@
         <v>280</v>
       </c>
       <c r="B120" s="16" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C120" s="16" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D120" s="16" t="s">
         <v>16</v>
@@ -4952,10 +4924,10 @@
         <v>280</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C121" s="16" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D121" s="16" t="s">
         <v>16</v>
@@ -4985,10 +4957,10 @@
         <v>280</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C122" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D122" s="16" t="s">
         <v>16</v>
@@ -5018,10 +4990,10 @@
         <v>280</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C123" s="16" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D123" s="16" t="s">
         <v>16</v>
@@ -5051,10 +5023,10 @@
         <v>280</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C124" s="16" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D124" s="16" t="s">
         <v>16</v>
@@ -5084,10 +5056,10 @@
         <v>280</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C125" s="16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D125" s="16" t="s">
         <v>16</v>
@@ -5117,10 +5089,10 @@
         <v>280</v>
       </c>
       <c r="B126" s="18" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D126" s="16" t="s">
         <v>16</v>
@@ -5150,10 +5122,10 @@
         <v>280</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C127" s="16" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D127" s="16" t="s">
         <v>16</v>
@@ -5183,10 +5155,10 @@
         <v>280</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D128" s="16" t="s">
         <v>16</v>
@@ -5216,10 +5188,10 @@
         <v>280</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C129" s="16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D129" s="16" t="s">
         <v>16</v>
@@ -5249,10 +5221,10 @@
         <v>280</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C130" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D130" s="16" t="s">
         <v>16</v>
@@ -5282,10 +5254,10 @@
         <v>280</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C131" s="16" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D131" s="16" t="s">
         <v>16</v>
@@ -5315,10 +5287,10 @@
         <v>280</v>
       </c>
       <c r="B132" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C132" s="16" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D132" s="16" t="s">
         <v>16</v>
@@ -5348,10 +5320,10 @@
         <v>280</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C133" s="16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D133" s="16" t="s">
         <v>16</v>
@@ -5381,10 +5353,10 @@
         <v>280</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C134" s="16" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D134" s="16" t="s">
         <v>16</v>
@@ -5414,10 +5386,10 @@
         <v>280</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C135" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D135" s="16" t="s">
         <v>16</v>
@@ -5444,13 +5416,13 @@
     </row>
     <row r="136" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C136" s="4" t="s">
         <v>323</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>325</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>16</v>
@@ -5461,10 +5433,10 @@
         <v>280</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C137" s="16" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D137" s="16" t="s">
         <v>16</v>
@@ -5492,10 +5464,10 @@
         <v>280</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C138" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D138" s="16" t="s">
         <v>77</v>
@@ -5523,10 +5495,10 @@
         <v>280</v>
       </c>
       <c r="B139" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C139" s="16" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D139" s="16" t="s">
         <v>16</v>
@@ -5554,10 +5526,10 @@
         <v>280</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C140" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D140" s="16" t="s">
         <v>16</v>
@@ -5585,10 +5557,10 @@
         <v>280</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C141" s="16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D141" s="16" t="s">
         <v>16</v>
@@ -5616,10 +5588,10 @@
         <v>280</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C142" s="16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D142" s="16" t="s">
         <v>16</v>
@@ -5647,10 +5619,10 @@
         <v>280</v>
       </c>
       <c r="B143" s="16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C143" s="16" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D143" s="16" t="s">
         <v>77</v>
@@ -5674,21 +5646,11 @@
       <c r="S143" s="16"/>
     </row>
     <row r="144" spans="1:21" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="16" t="s">
-        <v>280</v>
-      </c>
-      <c r="B144" s="16" t="s">
-        <v>340</v>
-      </c>
-      <c r="C144" s="16" t="s">
-        <v>341</v>
-      </c>
-      <c r="D144" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E144" s="16">
-        <v>1</v>
-      </c>
+      <c r="A144" s="16"/>
+      <c r="B144" s="16"/>
+      <c r="C144" s="16"/>
+      <c r="D144" s="16"/>
+      <c r="E144" s="16"/>
       <c r="F144" s="12"/>
       <c r="G144" s="16"/>
       <c r="H144" s="12"/>
@@ -5709,10 +5671,10 @@
         <v>280</v>
       </c>
       <c r="B145" s="16" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C145" s="16" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D145" s="16" t="s">
         <v>16</v>
@@ -5740,10 +5702,10 @@
         <v>280</v>
       </c>
       <c r="B146" s="16" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C146" s="16" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D146" s="16" t="s">
         <v>16</v>
@@ -5771,10 +5733,10 @@
         <v>280</v>
       </c>
       <c r="B147" s="16" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C147" s="16" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D147" s="16" t="s">
         <v>16</v>
@@ -5802,10 +5764,10 @@
         <v>280</v>
       </c>
       <c r="B148" s="16" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C148" s="16" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D148" s="16" t="s">
         <v>16</v>
@@ -5833,10 +5795,10 @@
         <v>280</v>
       </c>
       <c r="B149" s="16" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C149" s="16" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D149" s="16" t="s">
         <v>16</v>
@@ -5864,10 +5826,10 @@
         <v>280</v>
       </c>
       <c r="B150" s="16" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C150" s="16" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D150" s="16" t="s">
         <v>16</v>
@@ -5895,10 +5857,10 @@
         <v>280</v>
       </c>
       <c r="B151" s="16" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C151" s="16" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D151" s="16" t="s">
         <v>16</v>
@@ -5926,10 +5888,10 @@
         <v>280</v>
       </c>
       <c r="B152" s="16" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C152" s="16" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D152" s="16" t="s">
         <v>16</v>
@@ -5957,10 +5919,10 @@
         <v>280</v>
       </c>
       <c r="B153" s="16" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C153" s="16" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D153" s="16" t="s">
         <v>16</v>
@@ -5988,10 +5950,10 @@
         <v>280</v>
       </c>
       <c r="B154" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C154" s="16" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D154" s="16" t="s">
         <v>16</v>
@@ -6019,10 +5981,10 @@
         <v>280</v>
       </c>
       <c r="B155" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C155" s="16" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D155" s="16" t="s">
         <v>16</v>
@@ -6050,10 +6012,10 @@
         <v>280</v>
       </c>
       <c r="B156" s="16" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C156" s="16" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D156" s="16" t="s">
         <v>16</v>
@@ -6081,10 +6043,10 @@
         <v>280</v>
       </c>
       <c r="B157" s="16" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C157" s="16" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D157" s="16" t="s">
         <v>16</v>
@@ -6112,10 +6074,10 @@
         <v>280</v>
       </c>
       <c r="B158" s="16" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C158" s="16" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D158" s="16" t="s">
         <v>16</v>
@@ -6143,10 +6105,10 @@
         <v>280</v>
       </c>
       <c r="B159" s="16" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C159" s="16" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D159" s="16" t="s">
         <v>16</v>
@@ -6174,10 +6136,10 @@
         <v>280</v>
       </c>
       <c r="B160" s="16" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C160" s="16" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D160" s="16" t="s">
         <v>16</v>
@@ -6205,10 +6167,10 @@
         <v>280</v>
       </c>
       <c r="B161" s="16" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C161" s="16" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D161" s="16" t="s">
         <v>16</v>
@@ -6236,10 +6198,10 @@
         <v>280</v>
       </c>
       <c r="B162" s="16" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D162" s="16" t="s">
         <v>16</v>
@@ -6250,10 +6212,10 @@
     </row>
     <row r="163" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="16" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C163" s="4"/>
       <c r="D163" s="16" t="s">
@@ -6263,7 +6225,7 @@
         <v>1</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="164" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -6271,13 +6233,13 @@
         <v>72</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C164" s="11" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E164" s="1">
         <v>3</v>
@@ -6295,13 +6257,13 @@
         <v>72</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C165" s="11" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E165" s="1">
         <v>3</v>
@@ -6315,13 +6277,13 @@
         <v>72</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C166" s="11" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E166" s="1">
         <v>3</v>
@@ -6338,13 +6300,13 @@
         <v>72</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C167" s="11" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E167" s="1">
         <v>2</v>
@@ -6365,13 +6327,13 @@
         <v>72</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C168" s="11" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E168" s="1">
         <v>2</v>
@@ -6392,13 +6354,13 @@
         <v>72</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C169" s="11" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E169" s="1">
         <v>1</v>
@@ -6419,13 +6381,13 @@
         <v>72</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C170" s="11" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E170" s="1">
         <v>1</v>
@@ -6443,13 +6405,13 @@
         <v>72</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C171" s="11" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E171" s="1">
         <v>1</v>
@@ -6467,13 +6429,13 @@
         <v>72</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C172" s="11" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E172" s="1">
         <v>1</v>
@@ -6491,13 +6453,13 @@
         <v>72</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C173" s="11" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E173" s="1">
         <v>2</v>
@@ -6515,13 +6477,13 @@
         <v>72</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C174" s="11" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E174" s="1">
         <v>1</v>
@@ -6539,13 +6501,13 @@
         <v>72</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C175" s="11" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E175" s="1">
         <v>1</v>
@@ -6561,13 +6523,13 @@
     <row r="176" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1"/>
       <c r="B176" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C176" s="11" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E176" s="1">
         <v>1</v>
@@ -6585,13 +6547,13 @@
         <v>72</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C177" s="11" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E177" s="1">
         <v>1</v>
@@ -6604,13 +6566,13 @@
         <v>72</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C178" s="11" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E178" s="1">
         <v>1</v>
@@ -6623,10 +6585,10 @@
         <v>72</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C179" s="11" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>16</v>
@@ -6647,10 +6609,10 @@
         <v>72</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C180" s="11" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>16</v>
@@ -6664,10 +6626,10 @@
         <v>72</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C181" s="11" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>16</v>
@@ -6678,13 +6640,13 @@
     </row>
     <row r="182" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>16</v>
@@ -6698,13 +6660,13 @@
     </row>
     <row r="183" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>16</v>
@@ -6721,19 +6683,26 @@
         <v>13</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E184" s="2">
-        <v>1</v>
-      </c>
-      <c r="F184" s="2" t="s">
-        <v>424</v>
+        <v>2</v>
+      </c>
+      <c r="F184" s="20">
+        <f>H184*E184</f>
+        <v>1449.52</v>
+      </c>
+      <c r="G184" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H184" s="1">
+        <v>724.76</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -6741,10 +6710,10 @@
         <v>13</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C185" s="11" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>16</v>
@@ -6762,16 +6731,16 @@
     </row>
     <row r="186" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="C186" s="11" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="E186" s="1">
         <v>1</v>
@@ -6782,16 +6751,16 @@
     </row>
     <row r="187" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C187" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="B187" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C187" s="11" t="s">
-        <v>432</v>
-      </c>
       <c r="D187" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="E187" s="1">
         <v>1</v>
@@ -6808,7 +6777,7 @@
         <v>84889</v>
       </c>
       <c r="C188" s="11" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>47</v>
@@ -6829,10 +6798,10 @@
         <v>13</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>47</v>
@@ -6841,7 +6810,7 @@
         <v>1</v>
       </c>
       <c r="F189" s="2" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="190" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -6849,10 +6818,10 @@
         <v>13</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C190" s="11" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>33</v>
@@ -6870,13 +6839,13 @@
     </row>
     <row r="191" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="C191" s="11" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>16</v>
@@ -6893,186 +6862,186 @@
     </row>
     <row r="192" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C192" s="11" t="s">
         <v>439</v>
       </c>
-      <c r="B192" s="1" t="s">
+      <c r="D192" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E192" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E193" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C194" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="C192" s="11" t="s">
+      <c r="D194" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E194" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B195" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="D192" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E192" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B193" s="1" t="s">
+      <c r="C195" s="11" t="s">
         <v>445</v>
       </c>
-      <c r="C193" s="4" t="s">
+      <c r="D195" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E195" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="D193" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E193" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B194" s="1" t="s">
+      <c r="C196" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="C194" s="11" t="s">
+      <c r="D196" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E196" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B197" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="D194" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E194" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B195" s="1" t="s">
+      <c r="C197" s="11" t="s">
         <v>449</v>
       </c>
-      <c r="C195" s="11" t="s">
+      <c r="D197" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E197" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B198" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="D195" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E195" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B196" s="1" t="s">
+      <c r="C198" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="C196" s="11" t="s">
+      <c r="D198" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E198" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B199" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="D196" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E196" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B197" s="1" t="s">
+      <c r="C199" s="11" t="s">
         <v>453</v>
       </c>
-      <c r="C197" s="11" t="s">
+      <c r="D199" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="D197" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E197" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="C198" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="D198" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E198" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="C199" s="11" t="s">
-        <v>458</v>
-      </c>
-      <c r="D199" s="1" t="s">
-        <v>459</v>
       </c>
       <c r="E199" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B200" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C200" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E200" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C201" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E201" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C202" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="C200" s="11" t="s">
+      <c r="D202" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="D200" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E200" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="201" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C201" s="11" t="s">
-        <v>463</v>
-      </c>
-      <c r="D201" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="E201" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A202" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="C202" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="D202" s="1" t="s">
-        <v>466</v>
       </c>
       <c r="E202" s="1">
         <v>1</v>
@@ -7080,19 +7049,22 @@
       <c r="F202" s="1">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J202" s="19" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B203" s="1">
         <v>16399</v>
       </c>
       <c r="C203" s="11" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E203" s="1">
         <v>1</v>
@@ -7100,50 +7072,53 @@
       <c r="F203" s="1">
         <v>82.76</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J203" s="19" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C204" s="11" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E204" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="C205" s="11" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E205" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C206" s="11" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>16</v>
@@ -7159,18 +7134,18 @@
         <v>72.760000000000005</v>
       </c>
       <c r="I206" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="207" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B207" s="7" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>16</v>
@@ -7186,15 +7161,15 @@
         <v>31.117000000000001</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C208" s="11" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D208" s="1" t="s">
         <v>16</v>
@@ -7215,20 +7190,20 @@
         <v>13</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C209" s="11" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E209" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F209" s="1">
         <f t="shared" si="16"/>
-        <v>53.37</v>
+        <v>106.74</v>
       </c>
       <c r="H209" s="1">
         <v>53.37</v>
@@ -7239,10 +7214,10 @@
         <v>222</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="C210" s="11" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="D210" s="1" t="s">
         <v>16</v>
@@ -7258,7 +7233,7 @@
         <v>72.760000000000005</v>
       </c>
       <c r="I210" s="2" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="211" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -7266,10 +7241,10 @@
         <v>13</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="C211" s="11" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>16</v>
@@ -7287,16 +7262,16 @@
     </row>
     <row r="212" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="C212" s="11" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E212" s="1">
         <v>20</v>
@@ -7314,16 +7289,16 @@
     </row>
     <row r="213" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="C213" s="11" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E213" s="1">
         <v>120</v>
@@ -7341,16 +7316,16 @@
     </row>
     <row r="214" spans="1:21" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="12" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B214" s="12" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="C214" s="13" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D214" s="12" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E214" s="12">
         <v>0</v>
@@ -7381,16 +7356,16 @@
     </row>
     <row r="215" spans="1:21" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="12" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B215" s="12" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="C215" s="13" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D215" s="12" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E215" s="12">
         <v>20</v>
@@ -7408,16 +7383,16 @@
     </row>
     <row r="216" spans="1:21" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="12" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B216" s="12" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="D216" s="12" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E216" s="12">
         <v>0</v>
@@ -7448,16 +7423,16 @@
     </row>
     <row r="217" spans="1:21" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="12" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B217" s="12" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="C217" s="13" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="D217" s="12" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E217" s="12">
         <v>0</v>
@@ -7488,19 +7463,19 @@
     </row>
     <row r="218" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="C218" s="11" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="D218" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="F218" s="1">
         <v>66</v>
@@ -7515,16 +7490,16 @@
     </row>
     <row r="219" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="C219" s="11" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E219" s="1">
         <v>20</v>
@@ -7542,19 +7517,19 @@
     </row>
     <row r="220" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="D220" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E220" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F220" s="2">
         <v>366.84</v>
@@ -7564,38 +7539,18 @@
       </c>
     </row>
     <row r="221" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B221" s="2">
-        <v>16399</v>
-      </c>
-      <c r="C221" s="4" t="s">
-        <v>510</v>
-      </c>
-      <c r="D221" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="E221" s="2">
-        <v>1</v>
-      </c>
+      <c r="A221" s="1"/>
+      <c r="B221" s="2"/>
+      <c r="C221" s="4"/>
+      <c r="D221" s="2"/>
+      <c r="E221" s="2"/>
     </row>
     <row r="222" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B222" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="C222" s="11" t="s">
-        <v>512</v>
-      </c>
-      <c r="D222" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="E222" s="2">
-        <v>1</v>
-      </c>
+      <c r="A222" s="1"/>
+      <c r="B222" s="2"/>
+      <c r="C222" s="11"/>
+      <c r="D222" s="2"/>
+      <c r="E222" s="2"/>
     </row>
     <row r="223" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C223" s="11"/>
@@ -9794,6 +9749,10 @@
       <c r="C954" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J202" r:id="rId1"/>
+    <hyperlink ref="J203" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the dicrhoic filters to the latest
</commit_message>
<xml_diff>
--- a/PartsList.xlsx
+++ b/PartsList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/engs1793_ox_ac_uk/Documents/4pi_workspace/Git/CAD-files_JW/CAD-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_24B83572BA8ADC7BFD66B936B856E04174FEF458" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{19C7C836-5B6D-4C6A-B1DA-F994209AC83A}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_24B83572BA8ADC7BFD66B936B856E04174FEF458" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{C5CB738C-D8A1-4345-A334-2401C2CB97BB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4Pi-SMS part list" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="503">
   <si>
     <t>Category</t>
   </si>
@@ -795,12 +795,6 @@
     <t>Semrock</t>
   </si>
   <si>
-    <t xml:space="preserve">Di01-R405/488/561/635-17.5x24 </t>
-  </si>
-  <si>
-    <t>405/488/561/635 BrightLine Laser Dichroic Beam splitter, 17.5 x 24.0 mm</t>
-  </si>
-  <si>
     <t>DI0 and DI1</t>
   </si>
   <si>
@@ -816,16 +810,10 @@
     <t>Chroma</t>
   </si>
   <si>
-    <t>EM filters</t>
-  </si>
-  <si>
     <t>FF01-600/52-25</t>
   </si>
   <si>
     <t>600/52 nm BrightLine® single-band bandpass filter</t>
-  </si>
-  <si>
-    <t>Optics-excitation</t>
   </si>
   <si>
     <t>FF01-390/482/563/640-25</t>
@@ -1536,12 +1524,6 @@
     <t>Consumables</t>
   </si>
   <si>
-    <t>ZT405/488/561/640rpc</t>
-  </si>
-  <si>
-    <t>Filters</t>
-  </si>
-  <si>
     <t>ZET405/488/561/640mv2</t>
   </si>
   <si>
@@ -1552,6 +1534,12 @@
   </si>
   <si>
     <t>LS1</t>
+  </si>
+  <si>
+    <t>ZT405/488/561/640rpcv2-UF1</t>
+  </si>
+  <si>
+    <t>405/488/561/640 Laser Dichroic Beam splitter, 17.5 x 24.0 mm</t>
   </si>
 </sst>
 </file>
@@ -1866,8 +1854,8 @@
   <dimension ref="A1:R955"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C188" sqref="C188"/>
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3830,20 +3818,16 @@
       </c>
     </row>
     <row r="107" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>501</v>
-      </c>
+      <c r="A107" s="3"/>
+      <c r="B107" s="1"/>
       <c r="C107" s="2"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="3"/>
     </row>
     <row r="108" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>212</v>
+      <c r="A108" s="3" t="s">
+        <v>256</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>252</v>
@@ -3859,37 +3843,37 @@
       </c>
     </row>
     <row r="109" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>212</v>
+      <c r="A109" s="3" t="s">
+        <v>256</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>255</v>
+        <v>501</v>
       </c>
       <c r="C109" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>254</v>
+        <v>502</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>259</v>
       </c>
       <c r="E109" s="1">
         <v>2</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C110" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="D110" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="E110" s="3">
         <v>1</v>
@@ -3898,16 +3882,16 @@
     </row>
     <row r="111" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E111" s="3">
         <v>2</v>
@@ -3916,13 +3900,13 @@
     </row>
     <row r="112" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>254</v>
@@ -3932,14 +3916,14 @@
       </c>
     </row>
     <row r="113" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="15" t="s">
-        <v>265</v>
+      <c r="A113" s="3" t="s">
+        <v>256</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C113" s="16" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D113" s="12" t="s">
         <v>254</v>
@@ -3948,7 +3932,7 @@
         <v>1</v>
       </c>
       <c r="F113" s="15" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G113" s="12"/>
       <c r="H113" s="12"/>
@@ -3965,13 +3949,13 @@
     </row>
     <row r="114" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D114" s="15" t="s">
         <v>9</v>
@@ -3995,13 +3979,13 @@
     </row>
     <row r="115" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="B115" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="C115" s="15" t="s">
         <v>269</v>
-      </c>
-      <c r="B115" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="C115" s="15" t="s">
-        <v>273</v>
       </c>
       <c r="D115" s="15" t="s">
         <v>9</v>
@@ -4025,13 +4009,13 @@
     </row>
     <row r="116" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B116" s="15" t="s">
         <v>48</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D116" s="15" t="s">
         <v>9</v>
@@ -4055,13 +4039,13 @@
     </row>
     <row r="117" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D117" s="15" t="s">
         <v>9</v>
@@ -4085,13 +4069,13 @@
     </row>
     <row r="118" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D118" s="15" t="s">
         <v>9</v>
@@ -4115,13 +4099,13 @@
     </row>
     <row r="119" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D119" s="15" t="s">
         <v>9</v>
@@ -4145,13 +4129,13 @@
     </row>
     <row r="120" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D120" s="15" t="s">
         <v>9</v>
@@ -4175,13 +4159,13 @@
     </row>
     <row r="121" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D121" s="15" t="s">
         <v>9</v>
@@ -4205,13 +4189,13 @@
     </row>
     <row r="122" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B122" s="15" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D122" s="15" t="s">
         <v>9</v>
@@ -4235,13 +4219,13 @@
     </row>
     <row r="123" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B123" s="15" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D123" s="15" t="s">
         <v>9</v>
@@ -4265,13 +4249,13 @@
     </row>
     <row r="124" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B124" s="15" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D124" s="15" t="s">
         <v>9</v>
@@ -4295,13 +4279,13 @@
     </row>
     <row r="125" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B125" s="15" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D125" s="15" t="s">
         <v>9</v>
@@ -4325,13 +4309,13 @@
     </row>
     <row r="126" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B126" s="15" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D126" s="15" t="s">
         <v>9</v>
@@ -4355,13 +4339,13 @@
     </row>
     <row r="127" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B127" s="17" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D127" s="15" t="s">
         <v>9</v>
@@ -4385,13 +4369,13 @@
     </row>
     <row r="128" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B128" s="15" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D128" s="15" t="s">
         <v>9</v>
@@ -4415,13 +4399,13 @@
     </row>
     <row r="129" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B129" s="15" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D129" s="15" t="s">
         <v>9</v>
@@ -4445,13 +4429,13 @@
     </row>
     <row r="130" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B130" s="15" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D130" s="15" t="s">
         <v>9</v>
@@ -4475,13 +4459,13 @@
     </row>
     <row r="131" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B131" s="15" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D131" s="15" t="s">
         <v>9</v>
@@ -4505,13 +4489,13 @@
     </row>
     <row r="132" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B132" s="15" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D132" s="15" t="s">
         <v>9</v>
@@ -4535,13 +4519,13 @@
     </row>
     <row r="133" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B133" s="15" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D133" s="15" t="s">
         <v>9</v>
@@ -4565,13 +4549,13 @@
     </row>
     <row r="134" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B134" s="15" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D134" s="15" t="s">
         <v>9</v>
@@ -4595,13 +4579,13 @@
     </row>
     <row r="135" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B135" s="15" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D135" s="15" t="s">
         <v>9</v>
@@ -4625,13 +4609,13 @@
     </row>
     <row r="136" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B136" s="15" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D136" s="15" t="s">
         <v>9</v>
@@ -4655,13 +4639,13 @@
     </row>
     <row r="137" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>9</v>
@@ -4669,13 +4653,13 @@
     </row>
     <row r="138" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B138" s="15" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D138" s="15" t="s">
         <v>9</v>
@@ -4697,13 +4681,13 @@
     </row>
     <row r="139" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B139" s="15" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D139" s="15" t="s">
         <v>70</v>
@@ -4725,13 +4709,13 @@
     </row>
     <row r="140" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B140" s="15" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D140" s="15" t="s">
         <v>9</v>
@@ -4753,13 +4737,13 @@
     </row>
     <row r="141" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B141" s="15" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D141" s="15" t="s">
         <v>9</v>
@@ -4781,13 +4765,13 @@
     </row>
     <row r="142" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B142" s="15" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D142" s="15" t="s">
         <v>9</v>
@@ -4809,13 +4793,13 @@
     </row>
     <row r="143" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B143" s="15" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D143" s="15" t="s">
         <v>9</v>
@@ -4837,13 +4821,13 @@
     </row>
     <row r="144" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B144" s="15" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D144" s="15" t="s">
         <v>70</v>
@@ -4865,13 +4849,13 @@
     </row>
     <row r="145" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B145" s="15" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D145" s="15" t="s">
         <v>9</v>
@@ -4893,13 +4877,13 @@
     </row>
     <row r="146" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B146" s="15" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D146" s="15" t="s">
         <v>9</v>
@@ -4921,13 +4905,13 @@
     </row>
     <row r="147" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B147" s="15" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D147" s="15" t="s">
         <v>9</v>
@@ -4949,13 +4933,13 @@
     </row>
     <row r="148" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B148" s="15" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D148" s="15" t="s">
         <v>9</v>
@@ -4977,13 +4961,13 @@
     </row>
     <row r="149" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B149" s="15" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D149" s="15" t="s">
         <v>9</v>
@@ -5005,13 +4989,13 @@
     </row>
     <row r="150" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B150" s="15" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D150" s="15" t="s">
         <v>9</v>
@@ -5033,13 +5017,13 @@
     </row>
     <row r="151" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B151" s="15" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D151" s="15" t="s">
         <v>9</v>
@@ -5061,13 +5045,13 @@
     </row>
     <row r="152" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B152" s="15" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D152" s="15" t="s">
         <v>9</v>
@@ -5089,13 +5073,13 @@
     </row>
     <row r="153" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D153" s="15" t="s">
         <v>9</v>
@@ -5117,13 +5101,13 @@
     </row>
     <row r="154" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B154" s="15" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D154" s="15" t="s">
         <v>9</v>
@@ -5145,13 +5129,13 @@
     </row>
     <row r="155" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B155" s="15" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D155" s="15" t="s">
         <v>9</v>
@@ -5173,13 +5157,13 @@
     </row>
     <row r="156" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B156" s="15" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D156" s="15" t="s">
         <v>9</v>
@@ -5201,13 +5185,13 @@
     </row>
     <row r="157" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D157" s="15" t="s">
         <v>9</v>
@@ -5229,13 +5213,13 @@
     </row>
     <row r="158" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B158" s="15" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D158" s="15" t="s">
         <v>9</v>
@@ -5257,13 +5241,13 @@
     </row>
     <row r="159" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B159" s="15" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D159" s="15" t="s">
         <v>9</v>
@@ -5285,13 +5269,13 @@
     </row>
     <row r="160" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B160" s="15" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D160" s="15" t="s">
         <v>9</v>
@@ -5313,13 +5297,13 @@
     </row>
     <row r="161" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B161" s="15" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D161" s="15" t="s">
         <v>9</v>
@@ -5341,13 +5325,13 @@
     </row>
     <row r="162" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B162" s="15" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D162" s="15" t="s">
         <v>9</v>
@@ -5369,13 +5353,13 @@
     </row>
     <row r="163" spans="1:16" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B163" s="15" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D163" s="15" t="s">
         <v>9</v>
@@ -5386,10 +5370,10 @@
     </row>
     <row r="164" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="15" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C164" s="5"/>
       <c r="D164" s="15" t="s">
@@ -5399,7 +5383,7 @@
         <v>1</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="165" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5407,13 +5391,13 @@
         <v>65</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E165" s="1">
         <v>3</v>
@@ -5424,13 +5408,13 @@
         <v>65</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E166" s="1">
         <v>3</v>
@@ -5441,13 +5425,13 @@
         <v>65</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E167" s="1">
         <v>3</v>
@@ -5458,13 +5442,13 @@
         <v>65</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E168" s="1">
         <v>2</v>
@@ -5475,13 +5459,13 @@
         <v>65</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E169" s="1">
         <v>2</v>
@@ -5492,13 +5476,13 @@
         <v>65</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E170" s="1">
         <v>1</v>
@@ -5509,13 +5493,13 @@
         <v>65</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E171" s="1">
         <v>1</v>
@@ -5526,13 +5510,13 @@
         <v>65</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E172" s="1">
         <v>1</v>
@@ -5543,13 +5527,13 @@
         <v>65</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E173" s="1">
         <v>1</v>
@@ -5560,13 +5544,13 @@
         <v>65</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E174" s="1">
         <v>2</v>
@@ -5577,13 +5561,13 @@
         <v>65</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E175" s="1">
         <v>1</v>
@@ -5594,13 +5578,13 @@
         <v>65</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E176" s="1">
         <v>1</v>
@@ -5611,13 +5595,13 @@
         <v>65</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E177" s="1">
         <v>1</v>
@@ -5628,13 +5612,13 @@
         <v>65</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E178" s="1">
         <v>1</v>
@@ -5645,13 +5629,13 @@
         <v>65</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E179" s="1">
         <v>1</v>
@@ -5662,10 +5646,10 @@
         <v>65</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>9</v>
@@ -5679,10 +5663,10 @@
         <v>65</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>9</v>
@@ -5696,10 +5680,10 @@
         <v>65</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>9</v>
@@ -5710,13 +5694,13 @@
     </row>
     <row r="183" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>9</v>
@@ -5725,18 +5709,18 @@
         <v>1</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>9</v>
@@ -5745,7 +5729,7 @@
         <v>1</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5753,10 +5737,10 @@
         <v>6</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>9</v>
@@ -5770,10 +5754,10 @@
         <v>6</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>9</v>
@@ -5784,16 +5768,16 @@
     </row>
     <row r="187" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E187" s="1">
         <v>1</v>
@@ -5801,16 +5785,16 @@
     </row>
     <row r="188" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B188" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B188" s="1" t="s">
-        <v>419</v>
-      </c>
       <c r="C188" s="2" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E188" s="1">
         <v>1</v>
@@ -5824,7 +5808,7 @@
         <v>84889</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>40</v>
@@ -5838,10 +5822,10 @@
         <v>6</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>40</v>
@@ -5855,10 +5839,10 @@
         <v>6</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>26</v>
@@ -5869,13 +5853,13 @@
     </row>
     <row r="192" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>9</v>
@@ -5886,16 +5870,16 @@
     </row>
     <row r="193" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B193" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="B193" s="1" t="s">
-        <v>430</v>
-      </c>
       <c r="C193" s="2" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E193" s="1">
         <v>1</v>
@@ -5903,16 +5887,16 @@
     </row>
     <row r="194" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E194" s="1">
         <v>1</v>
@@ -5920,16 +5904,16 @@
     </row>
     <row r="195" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E195" s="1">
         <v>1</v>
@@ -5937,16 +5921,16 @@
     </row>
     <row r="196" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E196" s="1">
         <v>1</v>
@@ -5954,16 +5938,16 @@
     </row>
     <row r="197" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E197" s="1">
         <v>1</v>
@@ -5971,16 +5955,16 @@
     </row>
     <row r="198" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E198" s="1">
         <v>1</v>
@@ -5988,16 +5972,16 @@
     </row>
     <row r="199" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E199" s="1">
         <v>1</v>
@@ -6005,16 +5989,16 @@
     </row>
     <row r="200" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C200" s="18" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D200" s="18" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="E200" s="1">
         <v>2</v>
@@ -6022,16 +6006,16 @@
     </row>
     <row r="201" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E201" s="1">
         <v>1</v>
@@ -6039,16 +6023,16 @@
     </row>
     <row r="202" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E202" s="1">
         <v>1</v>
@@ -6056,16 +6040,16 @@
     </row>
     <row r="203" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="E203" s="1">
         <v>1</v>
@@ -6073,16 +6057,16 @@
     </row>
     <row r="204" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B204" s="1">
         <v>16399</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="E204" s="1">
         <v>1</v>
@@ -6090,16 +6074,16 @@
     </row>
     <row r="205" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C205" s="18" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E205" s="1">
         <v>4</v>
@@ -6107,16 +6091,16 @@
     </row>
     <row r="206" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C206" s="18" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E206" s="1">
         <v>1</v>
@@ -6127,10 +6111,10 @@
         <v>212</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>9</v>
@@ -6139,7 +6123,7 @@
         <v>3</v>
       </c>
       <c r="F207" s="3" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6147,10 +6131,10 @@
         <v>212</v>
       </c>
       <c r="B208" s="10" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C208" s="5" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D208" s="1" t="s">
         <v>9</v>
@@ -6164,10 +6148,10 @@
         <v>6</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>9</v>
@@ -6181,10 +6165,10 @@
         <v>6</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D210" s="1" t="s">
         <v>9</v>
@@ -6198,10 +6182,10 @@
         <v>212</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>9</v>
@@ -6210,7 +6194,7 @@
         <v>1</v>
       </c>
       <c r="F211" s="3" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="212" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6218,10 +6202,10 @@
         <v>6</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D212" s="1" t="s">
         <v>9</v>
@@ -6232,16 +6216,16 @@
     </row>
     <row r="213" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="6" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E213" s="1">
         <v>20</v>
@@ -6249,16 +6233,16 @@
     </row>
     <row r="214" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="6" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E214" s="1">
         <v>120</v>
@@ -6266,16 +6250,16 @@
     </row>
     <row r="215" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="19" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B215" s="19" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C215" s="13" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="D215" s="12" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E215" s="12">
         <v>0</v>
@@ -6296,16 +6280,16 @@
     </row>
     <row r="216" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="19" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B216" s="19" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D216" s="12" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E216" s="12">
         <v>20</v>
@@ -6313,16 +6297,16 @@
     </row>
     <row r="217" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="19" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B217" s="19" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="C217" s="13" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D217" s="12" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E217" s="12">
         <v>0</v>
@@ -6343,16 +6327,16 @@
     </row>
     <row r="218" spans="1:18" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="19" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B218" s="19" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C218" s="13" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D218" s="12" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E218" s="12">
         <v>0</v>
@@ -6373,33 +6357,33 @@
     </row>
     <row r="219" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="220" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E220" s="1">
         <v>20</v>
@@ -6407,33 +6391,33 @@
     </row>
     <row r="221" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C221" s="5" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="222" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B222" s="3">
         <v>16399</v>
       </c>
       <c r="C222" s="5" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="E222" s="3">
         <v>1</v>
@@ -6441,16 +6425,16 @@
     </row>
     <row r="223" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C223" s="18" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="E223" s="3">
         <v>1</v>

</xml_diff>